<commit_message>
Now we can select different routing methods to label the results
</commit_message>
<xml_diff>
--- a/INT/results/final_results.xlsx
+++ b/INT/results/final_results.xlsx
@@ -7,7 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="LOW" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="LOW-KShort" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="LOW-ECMP" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="LOW-ECMP-SRv6" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -417,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -425,17 +427,17 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="14" customWidth="1" min="1" max="1"/>
+    <col width="30" customWidth="1" min="1" max="1"/>
     <col width="37" customWidth="1" min="2" max="2"/>
-    <col width="37" customWidth="1" min="3" max="3"/>
-    <col width="37" customWidth="1" min="4" max="4"/>
-    <col width="37" customWidth="1" min="5" max="5"/>
-    <col width="22" customWidth="1" min="6" max="6"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="9" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="5" max="5"/>
+    <col width="41" customWidth="1" min="6" max="6"/>
     <col width="27" customWidth="1" min="7" max="7"/>
     <col width="21" customWidth="1" min="8" max="8"/>
     <col width="5" customWidth="1" min="9" max="9"/>
     <col width="12" customWidth="1" min="10" max="10"/>
-    <col width="23" customWidth="1" min="11" max="11"/>
+    <col width="21" customWidth="1" min="11" max="11"/>
     <col width="16" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
@@ -467,7 +469,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>1º Packet (TimeStamp)</t>
+          <t>1º Packet Timestamp(seconds,miliseconds)</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -516,7 +518,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -524,10 +526,10 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="F4" t="n">
-        <v>1721585733.050748</v>
+        <v>1722085739.21441</v>
       </c>
     </row>
     <row r="5">
@@ -542,7 +544,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -550,10 +552,10 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="F5" t="n">
-        <v>1721585733.037938</v>
+        <v>1722085739.310087</v>
       </c>
       <c r="G5" t="n">
         <v>0</v>
@@ -576,209 +578,992 @@
         <v/>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+    <row r="6"/>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Iteration - 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
         <is>
           <t>2001:1:1::1</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2001:1:3::1</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>2</v>
-      </c>
-      <c r="D6" t="inlineStr">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2001:1:2::1</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="inlineStr">
         <is>
           <t>sender</t>
         </is>
       </c>
-      <c r="E6" t="n">
-        <v>10</v>
-      </c>
-      <c r="F6" t="n">
-        <v>1721586500.378799</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="E8" t="n">
+        <v>99</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1722085749.345705</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
         <is>
           <t>2001:1:1::1</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2001:1:3::1</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>2</v>
-      </c>
-      <c r="D7" t="inlineStr">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2001:1:2::1</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="inlineStr">
         <is>
           <t>receiver</t>
         </is>
       </c>
-      <c r="E7" t="n">
-        <v>10</v>
-      </c>
-      <c r="F7" t="n">
-        <v>1721586500.374454</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="J7">
-        <f>E6-E7</f>
-        <v/>
-      </c>
-      <c r="K7">
-        <f>ROUND(J7/E6*100, 3)</f>
-        <v/>
-      </c>
-      <c r="L7">
-        <f>F7-F6</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8"/>
-    <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>Iteration - 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2001:1:1::1</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>2001:1:3::1</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>2</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>sender</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>10</v>
-      </c>
-      <c r="F10" t="n">
-        <v>1721586375.922825</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2001:1:1::1</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>2001:1:3::1</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>2</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>receiver</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
-        <v>10</v>
-      </c>
-      <c r="F11" t="n">
-        <v>1721586375.913333</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
-      </c>
-      <c r="J11">
-        <f>E10-E11</f>
-        <v/>
-      </c>
-      <c r="K11">
-        <f>ROUND(J11/E10*100, 3)</f>
-        <v/>
-      </c>
-      <c r="L11">
-        <f>F11-F10</f>
-        <v/>
-      </c>
-    </row>
+      <c r="E9" t="n">
+        <v>84</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1722085743.385229</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="J9">
+        <f>E8-E9</f>
+        <v/>
+      </c>
+      <c r="K9">
+        <f>ROUND(J9/E8*100, 3)</f>
+        <v/>
+      </c>
+      <c r="L9">
+        <f>F9-F8</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10"/>
+    <row r="11"/>
     <row r="12"/>
-    <row r="13"/>
-    <row r="14"/>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>Calculations</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>Values</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>AVG Out of Order Packets (Nº)</t>
+        </is>
+      </c>
+      <c r="B14">
+        <f>ROUND(AVERAGEIF(G:G, "&lt;&gt;", G:G), 3)</f>
+        <v/>
+      </c>
+    </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Averages</t>
-        </is>
-      </c>
-      <c r="B15" s="1" t="inlineStr">
-        <is>
-          <t>Out of Order Packets (Nº)</t>
-        </is>
-      </c>
-      <c r="C15" s="1" t="inlineStr">
-        <is>
-          <t>Packet Loss (Nº)</t>
-        </is>
-      </c>
-      <c r="D15" s="1" t="inlineStr">
-        <is>
-          <t>Packet Loss (%)</t>
-        </is>
-      </c>
-      <c r="E15" s="1" t="inlineStr">
-        <is>
-          <t>1º Packet Delay</t>
-        </is>
+          <t>AVG Packet Loss (Nº)</t>
+        </is>
+      </c>
+      <c r="B15">
+        <f>ROUND(AVERAGEIF(J:J, "&lt;&gt;", J:J), 3)</f>
+        <v/>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
+          <t>AVG Packet Loss (%)</t>
+        </is>
+      </c>
+      <c r="B16">
+        <f>ROUND(AVERAGEIF(K:K, "&lt;&gt;", K:K), 3)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>AVG 1º Packet Delay</t>
+        </is>
+      </c>
+      <c r="B17">
+        <f>ROUND(AVERAGEIF(L:L, "&lt;&gt;", L:L), 3)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>AVG Flows Latency</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>7993.709292412617</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>AVG Processing Latency</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1998.427323103154</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>% of packets to each switch</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>Switch IDs</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Switch 1</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Switch 14</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Switch 2</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Switch 9</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="37" customWidth="1" min="2" max="2"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="9" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="5" max="5"/>
+    <col width="41" customWidth="1" min="6" max="6"/>
+    <col width="27" customWidth="1" min="7" max="7"/>
+    <col width="21" customWidth="1" min="8" max="8"/>
+    <col width="5" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+    <col width="21" customWidth="1" min="11" max="11"/>
+    <col width="16" customWidth="1" min="12" max="12"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Flow src</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Flow dst</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Flow Label</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Is</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Nº of packets</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>1º Packet Timestamp(seconds,miliseconds)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Nº of out of order packets</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Out of order packets</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Packet Loss</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Packet Loss (%)</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>1º Packet Delay</t>
+        </is>
+      </c>
+    </row>
+    <row r="2"/>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Iteration - 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2001:1:1::1</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2001:1:2::1</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>sender</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>99</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1722085767.48564</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2001:1:1::1</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2001:1:2::1</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>receiver</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>44</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1722085767.62095</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J5">
+        <f>E4-E5</f>
+        <v/>
+      </c>
+      <c r="K5">
+        <f>ROUND(J5/E4*100, 3)</f>
+        <v/>
+      </c>
+      <c r="L5">
+        <f>F5-F4</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6"/>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Iteration - 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2001:1:1::1</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2001:1:2::1</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>sender</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>99</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1722085777.641161</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2001:1:1::1</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2001:1:2::1</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>receiver</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>81</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1722085771.615925</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="J9">
+        <f>E8-E9</f>
+        <v/>
+      </c>
+      <c r="K9">
+        <f>ROUND(J9/E8*100, 3)</f>
+        <v/>
+      </c>
+      <c r="L9">
+        <f>F9-F8</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>Calculations</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
           <t>Values</t>
         </is>
       </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>AVG Out of Order Packets (Nº)</t>
+        </is>
+      </c>
+      <c r="B14">
+        <f>ROUND(AVERAGEIF(G:G, "&lt;&gt;", G:G), 3)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>AVG Packet Loss (Nº)</t>
+        </is>
+      </c>
+      <c r="B15">
+        <f>ROUND(AVERAGEIF(J:J, "&lt;&gt;", J:J), 3)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>AVG Packet Loss (%)</t>
+        </is>
+      </c>
       <c r="B16">
+        <f>ROUND(AVERAGEIF(K:K, "&lt;&gt;", K:K), 3)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>AVG 1º Packet Delay</t>
+        </is>
+      </c>
+      <c r="B17">
+        <f>ROUND(AVERAGEIF(L:L, "&lt;&gt;", L:L), 3)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>AVG Flows Latency</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>7993.709292412617</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>AVG Processing Latency</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1998.427323103154</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>% of packets to each switch</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>Switch IDs</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Switch 1</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Switch 14</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Switch 2</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Switch 9</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:L24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="30" customWidth="1" min="1" max="1"/>
+    <col width="37" customWidth="1" min="2" max="2"/>
+    <col width="11" customWidth="1" min="3" max="3"/>
+    <col width="9" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="5" max="5"/>
+    <col width="41" customWidth="1" min="6" max="6"/>
+    <col width="27" customWidth="1" min="7" max="7"/>
+    <col width="21" customWidth="1" min="8" max="8"/>
+    <col width="5" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+    <col width="21" customWidth="1" min="11" max="11"/>
+    <col width="16" customWidth="1" min="12" max="12"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Flow src</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Flow dst</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Flow Label</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Is</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Nº of packets</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>1º Packet Timestamp(seconds,miliseconds)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Nº of out of order packets</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Out of order packets</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Packet Loss</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Packet Loss (%)</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>1º Packet Delay</t>
+        </is>
+      </c>
+    </row>
+    <row r="2"/>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Iteration - 1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2001:1:1::1</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2001:1:2::1</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>sender</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>99</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1722085839.533898</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2001:1:1::1</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2001:1:2::1</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>receiver</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>43</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1722085839.659558</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="J5">
+        <f>E4-E5</f>
+        <v/>
+      </c>
+      <c r="K5">
+        <f>ROUND(J5/E4*100, 3)</f>
+        <v/>
+      </c>
+      <c r="L5">
+        <f>F5-F4</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6"/>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Iteration - 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2001:1:1::1</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2001:1:2::1</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>sender</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>99</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1722085849.839391</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2001:1:1::1</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2001:1:2::1</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>receiver</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>80</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1722085843.782593</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>[1]</t>
+        </is>
+      </c>
+      <c r="J9">
+        <f>E8-E9</f>
+        <v/>
+      </c>
+      <c r="K9">
+        <f>ROUND(J9/E8*100, 3)</f>
+        <v/>
+      </c>
+      <c r="L9">
+        <f>F9-F8</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>Calculations</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>Values</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>AVG Out of Order Packets (Nº)</t>
+        </is>
+      </c>
+      <c r="B14">
         <f>ROUND(AVERAGEIF(G:G, "&lt;&gt;", G:G), 3)</f>
         <v/>
       </c>
-      <c r="C16">
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>AVG Packet Loss (Nº)</t>
+        </is>
+      </c>
+      <c r="B15">
         <f>ROUND(AVERAGEIF(J:J, "&lt;&gt;", J:J), 3)</f>
         <v/>
       </c>
-      <c r="D16">
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>AVG Packet Loss (%)</t>
+        </is>
+      </c>
+      <c r="B16">
         <f>ROUND(AVERAGEIF(K:K, "&lt;&gt;", K:K), 3)</f>
         <v/>
       </c>
-      <c r="E16">
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>AVG 1º Packet Delay</t>
+        </is>
+      </c>
+      <c r="B17">
         <f>ROUND(AVERAGEIF(L:L, "&lt;&gt;", L:L), 3)</f>
         <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>AVG Flows Latency</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>7993.709292412617</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>AVG Processing Latency</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1998.427323103154</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>% of packets to each switch</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>Switch IDs</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Switch 1</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Switch 14</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Switch 2</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Switch 9</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
STD FLOW/HOP latency added to comparasions
</commit_message>
<xml_diff>
--- a/INT/results/final_results.xlsx
+++ b/INT/results/final_results.xlsx
@@ -4282,7 +4282,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4585,19 +4585,19 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>AVG Hop Latency (nanoseconds)</t>
+          <t>STD Flows Latency (nanoseconds)</t>
         </is>
       </c>
       <c r="B14">
-        <f>'MEDIUM-KShort'!B114</f>
+        <f>'MEDIUM-KShort'!B113</f>
         <v/>
       </c>
       <c r="C14">
-        <f>'MEDIUM-ECMP'!B114</f>
+        <f>'MEDIUM-ECMP'!B113</f>
         <v/>
       </c>
       <c r="D14">
-        <f>'MEDIUM-ECMP-SRv6'!B114</f>
+        <f>'MEDIUM-ECMP-SRv6'!B113</f>
         <v/>
       </c>
       <c r="E14">
@@ -4616,19 +4616,19 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>AVG of packets to each switch (%)</t>
+          <t>AVG Hop Latency (nanoseconds)</t>
         </is>
       </c>
       <c r="B15">
-        <f>'MEDIUM-KShort'!B126</f>
+        <f>'MEDIUM-KShort'!B114</f>
         <v/>
       </c>
       <c r="C15">
-        <f>'MEDIUM-ECMP'!B129</f>
+        <f>'MEDIUM-ECMP'!B114</f>
         <v/>
       </c>
       <c r="D15">
-        <f>'MEDIUM-ECMP-SRv6'!B128</f>
+        <f>'MEDIUM-ECMP-SRv6'!B114</f>
         <v/>
       </c>
       <c r="E15">
@@ -4647,19 +4647,19 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>Standard Deviation of packets to each switch (%)</t>
+          <t>STD Hop Latency (nanoseconds)</t>
         </is>
       </c>
       <c r="B16">
-        <f>'MEDIUM-KShort'!B127</f>
+        <f>'MEDIUM-KShort'!B115</f>
         <v/>
       </c>
       <c r="C16">
-        <f>'MEDIUM-ECMP'!B130</f>
+        <f>'MEDIUM-ECMP'!B115</f>
         <v/>
       </c>
       <c r="D16">
-        <f>'MEDIUM-ECMP-SRv6'!B129</f>
+        <f>'MEDIUM-ECMP-SRv6'!B115</f>
         <v/>
       </c>
       <c r="E16">
@@ -4678,7 +4678,7 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>AVG of processed Bytes to each switch</t>
+          <t>AVG of packets to each switch (%)</t>
         </is>
       </c>
       <c r="B17">
@@ -4709,7 +4709,7 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>Standard Deviation of processed Bytes to each switch</t>
+          <t>Standard Deviation of packets to each switch (%)</t>
         </is>
       </c>
       <c r="B18">
@@ -4740,19 +4740,19 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>Variation of the AVG 1º Packet Delay between (No)Emergency Flows (nanoseconds)</t>
+          <t>AVG of processed Bytes to each switch</t>
         </is>
       </c>
       <c r="B19">
-        <f>'MEDIUM-KShort'!D130</f>
+        <f>'MEDIUM-KShort'!C126</f>
         <v/>
       </c>
       <c r="C19">
-        <f>'MEDIUM-ECMP'!D133</f>
+        <f>'MEDIUM-ECMP'!C129</f>
         <v/>
       </c>
       <c r="D19">
-        <f>'MEDIUM-ECMP-SRv6'!D132</f>
+        <f>'MEDIUM-ECMP-SRv6'!C128</f>
         <v/>
       </c>
       <c r="E19">
@@ -4771,19 +4771,19 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Variation of the AVG Flow Delay between (No)Emergency Flows (nanoseconds)</t>
+          <t>Standard Deviation of processed Bytes to each switch</t>
         </is>
       </c>
       <c r="B20">
-        <f>'MEDIUM-KShort'!D131</f>
+        <f>'MEDIUM-KShort'!C127</f>
         <v/>
       </c>
       <c r="C20">
-        <f>'MEDIUM-ECMP'!D134</f>
+        <f>'MEDIUM-ECMP'!C130</f>
         <v/>
       </c>
       <c r="D20">
-        <f>'MEDIUM-ECMP-SRv6'!D133</f>
+        <f>'MEDIUM-ECMP-SRv6'!C129</f>
         <v/>
       </c>
       <c r="E20">
@@ -4799,123 +4799,123 @@
         <v/>
       </c>
     </row>
-    <row r="21"/>
-    <row r="22"/>
-    <row r="23">
-      <c r="A23" s="1" t="inlineStr">
-        <is>
-          <t>HIGH</t>
-        </is>
-      </c>
-      <c r="B23" s="1" t="inlineStr">
-        <is>
-          <t>KShort</t>
-        </is>
-      </c>
-      <c r="C23" s="1" t="inlineStr">
-        <is>
-          <t>ECMP</t>
-        </is>
-      </c>
-      <c r="D23" s="1" t="inlineStr">
-        <is>
-          <t>ECMP+SRv6</t>
-        </is>
-      </c>
-      <c r="E23" s="1" t="inlineStr">
-        <is>
-          <t>Variation1 (%)</t>
-        </is>
-      </c>
-      <c r="F23" s="1" t="inlineStr">
-        <is>
-          <t>Variation2 (%)</t>
-        </is>
-      </c>
-      <c r="G23" s="1" t="inlineStr">
-        <is>
-          <t>Variation3 (%)</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="inlineStr">
-        <is>
-          <t>AVG Out of Order Packets (Nº)</t>
-        </is>
-      </c>
-      <c r="B24">
-        <f>'HIGH-KShort'!B266</f>
-        <v/>
-      </c>
-      <c r="C24">
-        <f>'HIGH-ECMP'!B266</f>
-        <v/>
-      </c>
-      <c r="D24">
-        <f>'HIGH-ECMP-SRv6'!B327</f>
-        <v/>
-      </c>
-      <c r="E24">
-        <f>IFERROR(ROUND((C24 - B24) / B24 * 100, 3), 0)</f>
-        <v/>
-      </c>
-      <c r="F24">
-        <f>IFERROR(ROUND((D24 - B24) / B24 * 100, 3), 0)</f>
-        <v/>
-      </c>
-      <c r="G24">
-        <f>IFERROR(ROUND((D24 - C24) / C24 * 100, 3), 0)</f>
-        <v/>
-      </c>
-    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>Variation of the AVG 1º Packet Delay between (No)Emergency Flows (nanoseconds)</t>
+        </is>
+      </c>
+      <c r="B21">
+        <f>'MEDIUM-KShort'!D109</f>
+        <v/>
+      </c>
+      <c r="C21">
+        <f>'MEDIUM-ECMP'!D109</f>
+        <v/>
+      </c>
+      <c r="D21">
+        <f>'MEDIUM-ECMP-SRv6'!D109</f>
+        <v/>
+      </c>
+      <c r="E21">
+        <f>IFERROR(ROUND((C21 - B21) / B21 * 100, 3), 0)</f>
+        <v/>
+      </c>
+      <c r="F21">
+        <f>IFERROR(ROUND((D21 - B21) / B21 * 100, 3), 0)</f>
+        <v/>
+      </c>
+      <c r="G21">
+        <f>IFERROR(ROUND((D21 - C21) / C21 * 100, 3), 0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>Variation of the AVG Flow Delay between (No)Emergency Flows (nanoseconds)</t>
+        </is>
+      </c>
+      <c r="B22">
+        <f>'MEDIUM-KShort'!D131</f>
+        <v/>
+      </c>
+      <c r="C22">
+        <f>'MEDIUM-ECMP'!D134</f>
+        <v/>
+      </c>
+      <c r="D22">
+        <f>'MEDIUM-ECMP-SRv6'!D133</f>
+        <v/>
+      </c>
+      <c r="E22">
+        <f>IFERROR(ROUND((C22 - B22) / B22 * 100, 3), 0)</f>
+        <v/>
+      </c>
+      <c r="F22">
+        <f>IFERROR(ROUND((D22 - B22) / B22 * 100, 3), 0)</f>
+        <v/>
+      </c>
+      <c r="G22">
+        <f>IFERROR(ROUND((D22 - C22) / C22 * 100, 3), 0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23"/>
+    <row r="24"/>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>AVG Packet Loss (Nº)</t>
-        </is>
-      </c>
-      <c r="B25">
-        <f>'HIGH-KShort'!B267</f>
-        <v/>
-      </c>
-      <c r="C25">
-        <f>'HIGH-ECMP'!B267</f>
-        <v/>
-      </c>
-      <c r="D25">
-        <f>'HIGH-ECMP-SRv6'!B328</f>
-        <v/>
-      </c>
-      <c r="E25">
-        <f>IFERROR(ROUND((C25 - B25) / B25 * 100, 3), 0)</f>
-        <v/>
-      </c>
-      <c r="F25">
-        <f>IFERROR(ROUND((D25 - B25) / B25 * 100, 3), 0)</f>
-        <v/>
-      </c>
-      <c r="G25">
-        <f>IFERROR(ROUND((D25 - C25) / C25 * 100, 3), 0)</f>
-        <v/>
+          <t>HIGH</t>
+        </is>
+      </c>
+      <c r="B25" s="1" t="inlineStr">
+        <is>
+          <t>KShort</t>
+        </is>
+      </c>
+      <c r="C25" s="1" t="inlineStr">
+        <is>
+          <t>ECMP</t>
+        </is>
+      </c>
+      <c r="D25" s="1" t="inlineStr">
+        <is>
+          <t>ECMP+SRv6</t>
+        </is>
+      </c>
+      <c r="E25" s="1" t="inlineStr">
+        <is>
+          <t>Variation1 (%)</t>
+        </is>
+      </c>
+      <c r="F25" s="1" t="inlineStr">
+        <is>
+          <t>Variation2 (%)</t>
+        </is>
+      </c>
+      <c r="G25" s="1" t="inlineStr">
+        <is>
+          <t>Variation3 (%)</t>
+        </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>AVG Packet Loss (%)</t>
+          <t>AVG Out of Order Packets (Nº)</t>
         </is>
       </c>
       <c r="B26">
-        <f>'HIGH-KShort'!B268</f>
+        <f>'HIGH-KShort'!B266</f>
         <v/>
       </c>
       <c r="C26">
-        <f>'HIGH-ECMP'!B268</f>
+        <f>'HIGH-ECMP'!B266</f>
         <v/>
       </c>
       <c r="D26">
-        <f>'HIGH-ECMP-SRv6'!B329</f>
+        <f>'HIGH-ECMP-SRv6'!B327</f>
         <v/>
       </c>
       <c r="E26">
@@ -4934,19 +4934,19 @@
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>AVG 1º Packet Delay (nanoseconds)</t>
+          <t>AVG Packet Loss (Nº)</t>
         </is>
       </c>
       <c r="B27">
-        <f>'HIGH-KShort'!B269</f>
+        <f>'HIGH-KShort'!B267</f>
         <v/>
       </c>
       <c r="C27">
-        <f>'HIGH-ECMP'!B269</f>
+        <f>'HIGH-ECMP'!B267</f>
         <v/>
       </c>
       <c r="D27">
-        <f>'HIGH-ECMP-SRv6'!B330</f>
+        <f>'HIGH-ECMP-SRv6'!B328</f>
         <v/>
       </c>
       <c r="E27">
@@ -4965,19 +4965,19 @@
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>AVG Nº of SRv6 rules Created</t>
+          <t>AVG Packet Loss (%)</t>
         </is>
       </c>
       <c r="B28">
-        <f>'HIGH-KShort'!B270</f>
+        <f>'HIGH-KShort'!B268</f>
         <v/>
       </c>
       <c r="C28">
-        <f>'HIGH-ECMP'!B270</f>
+        <f>'HIGH-ECMP'!B268</f>
         <v/>
       </c>
       <c r="D28">
-        <f>'HIGH-ECMP-SRv6'!B331</f>
+        <f>'HIGH-ECMP-SRv6'!B329</f>
         <v/>
       </c>
       <c r="E28">
@@ -4996,19 +4996,19 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>AVG Nº of SRv6 rules Removed</t>
+          <t>AVG 1º Packet Delay (nanoseconds)</t>
         </is>
       </c>
       <c r="B29">
-        <f>'HIGH-KShort'!B271</f>
+        <f>'HIGH-KShort'!B269</f>
         <v/>
       </c>
       <c r="C29">
-        <f>'HIGH-ECMP'!B271</f>
+        <f>'HIGH-ECMP'!B269</f>
         <v/>
       </c>
       <c r="D29">
-        <f>'HIGH-ECMP-SRv6'!B332</f>
+        <f>'HIGH-ECMP-SRv6'!B330</f>
         <v/>
       </c>
       <c r="E29">
@@ -5027,19 +5027,19 @@
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>AVG Flows Latency (nanoseconds)</t>
+          <t>AVG Nº of SRv6 rules Created</t>
         </is>
       </c>
       <c r="B30">
-        <f>'HIGH-KShort'!B272</f>
+        <f>'HIGH-KShort'!B270</f>
         <v/>
       </c>
       <c r="C30">
-        <f>'HIGH-ECMP'!B272</f>
+        <f>'HIGH-ECMP'!B270</f>
         <v/>
       </c>
       <c r="D30">
-        <f>'HIGH-ECMP-SRv6'!B333</f>
+        <f>'HIGH-ECMP-SRv6'!B331</f>
         <v/>
       </c>
       <c r="E30">
@@ -5058,19 +5058,19 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>AVG Hop Latency (nanoseconds)</t>
+          <t>AVG Nº of SRv6 rules Removed</t>
         </is>
       </c>
       <c r="B31">
-        <f>'HIGH-KShort'!B274</f>
+        <f>'HIGH-KShort'!B271</f>
         <v/>
       </c>
       <c r="C31">
-        <f>'HIGH-ECMP'!B274</f>
+        <f>'HIGH-ECMP'!B271</f>
         <v/>
       </c>
       <c r="D31">
-        <f>'HIGH-ECMP-SRv6'!B335</f>
+        <f>'HIGH-ECMP-SRv6'!B332</f>
         <v/>
       </c>
       <c r="E31">
@@ -5089,19 +5089,19 @@
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>AVG of packets to each switch (%)</t>
+          <t>AVG Flows Latency (nanoseconds)</t>
         </is>
       </c>
       <c r="B32">
-        <f>'HIGH-KShort'!B288</f>
+        <f>'HIGH-KShort'!B272</f>
         <v/>
       </c>
       <c r="C32">
-        <f>'HIGH-ECMP'!B289</f>
+        <f>'HIGH-ECMP'!B272</f>
         <v/>
       </c>
       <c r="D32">
-        <f>'HIGH-ECMP-SRv6'!B351</f>
+        <f>'HIGH-ECMP-SRv6'!B333</f>
         <v/>
       </c>
       <c r="E32">
@@ -5120,19 +5120,19 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Standard Deviation of packets to each switch (%)</t>
+          <t>STD Flows Latency (nanoseconds)</t>
         </is>
       </c>
       <c r="B33">
-        <f>'HIGH-KShort'!B289</f>
+        <f>'HIGH-KShort'!B273</f>
         <v/>
       </c>
       <c r="C33">
-        <f>'HIGH-ECMP'!B290</f>
+        <f>'HIGH-ECMP'!B273</f>
         <v/>
       </c>
       <c r="D33">
-        <f>'HIGH-ECMP-SRv6'!B352</f>
+        <f>'HIGH-ECMP-SRv6'!B334</f>
         <v/>
       </c>
       <c r="E33">
@@ -5151,19 +5151,19 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>AVG of processed Bytes to each switch</t>
+          <t>AVG Hop Latency (nanoseconds)</t>
         </is>
       </c>
       <c r="B34">
-        <f>'HIGH-KShort'!C288</f>
+        <f>'HIGH-KShort'!B274</f>
         <v/>
       </c>
       <c r="C34">
-        <f>'HIGH-ECMP'!C289</f>
+        <f>'HIGH-ECMP'!B274</f>
         <v/>
       </c>
       <c r="D34">
-        <f>'HIGH-ECMP-SRv6'!C351</f>
+        <f>'HIGH-ECMP-SRv6'!B335</f>
         <v/>
       </c>
       <c r="E34">
@@ -5182,19 +5182,19 @@
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>Standard Deviation of processed Bytes to each switch</t>
+          <t>STD Hop Latency (nanoseconds)</t>
         </is>
       </c>
       <c r="B35">
-        <f>'HIGH-KShort'!C289</f>
+        <f>'HIGH-KShort'!B275</f>
         <v/>
       </c>
       <c r="C35">
-        <f>'HIGH-ECMP'!C290</f>
+        <f>'HIGH-ECMP'!B275</f>
         <v/>
       </c>
       <c r="D35">
-        <f>'HIGH-ECMP-SRv6'!C352</f>
+        <f>'HIGH-ECMP-SRv6'!B336</f>
         <v/>
       </c>
       <c r="E35">
@@ -5213,19 +5213,19 @@
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>Variation of the AVG 1º Packet Delay between (No)Emergency Flows (nanoseconds)</t>
+          <t>AVG of packets to each switch (%)</t>
         </is>
       </c>
       <c r="B36">
-        <f>'HIGH-KShort'!D292</f>
+        <f>'HIGH-KShort'!C288</f>
         <v/>
       </c>
       <c r="C36">
-        <f>'HIGH-ECMP'!D293</f>
+        <f>'HIGH-ECMP'!C289</f>
         <v/>
       </c>
       <c r="D36">
-        <f>'HIGH-ECMP-SRv6'!D355</f>
+        <f>'HIGH-ECMP-SRv6'!C351</f>
         <v/>
       </c>
       <c r="E36">
@@ -5244,19 +5244,19 @@
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>Variation of the AVG Flow Delay between (No)Emergency Flows (nanoseconds)</t>
+          <t>Standard Deviation of packets to each switch (%)</t>
         </is>
       </c>
       <c r="B37">
-        <f>'HIGH-KShort'!D293</f>
+        <f>'HIGH-KShort'!C289</f>
         <v/>
       </c>
       <c r="C37">
-        <f>'HIGH-ECMP'!D294</f>
+        <f>'HIGH-ECMP'!C290</f>
         <v/>
       </c>
       <c r="D37">
-        <f>'HIGH-ECMP-SRv6'!D356</f>
+        <f>'HIGH-ECMP-SRv6'!C352</f>
         <v/>
       </c>
       <c r="E37">
@@ -5272,61 +5272,115 @@
         <v/>
       </c>
     </row>
-    <row r="38"/>
-    <row r="39"/>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>AVG of processed Bytes to each switch</t>
+        </is>
+      </c>
+      <c r="B38">
+        <f>'HIGH-KShort'!C288</f>
+        <v/>
+      </c>
+      <c r="C38">
+        <f>'HIGH-ECMP'!C289</f>
+        <v/>
+      </c>
+      <c r="D38">
+        <f>'HIGH-ECMP-SRv6'!C351</f>
+        <v/>
+      </c>
+      <c r="E38">
+        <f>IFERROR(ROUND((C38 - B38) / B38 * 100, 3), 0)</f>
+        <v/>
+      </c>
+      <c r="F38">
+        <f>IFERROR(ROUND((D38 - B38) / B38 * 100, 3), 0)</f>
+        <v/>
+      </c>
+      <c r="G38">
+        <f>IFERROR(ROUND((D38 - C38) / C38 * 100, 3), 0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>Standard Deviation of processed Bytes to each switch</t>
+        </is>
+      </c>
+      <c r="B39">
+        <f>'HIGH-KShort'!C289</f>
+        <v/>
+      </c>
+      <c r="C39">
+        <f>'HIGH-ECMP'!C290</f>
+        <v/>
+      </c>
+      <c r="D39">
+        <f>'HIGH-ECMP-SRv6'!C352</f>
+        <v/>
+      </c>
+      <c r="E39">
+        <f>IFERROR(ROUND((C39 - B39) / B39 * 100, 3), 0)</f>
+        <v/>
+      </c>
+      <c r="F39">
+        <f>IFERROR(ROUND((D39 - B39) / B39 * 100, 3), 0)</f>
+        <v/>
+      </c>
+      <c r="G39">
+        <f>IFERROR(ROUND((D39 - C39) / C39 * 100, 3), 0)</f>
+        <v/>
+      </c>
+    </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>HIGH+EMERGENCY</t>
-        </is>
-      </c>
-      <c r="B40" s="1" t="inlineStr">
-        <is>
-          <t>KShort</t>
-        </is>
-      </c>
-      <c r="C40" s="1" t="inlineStr">
-        <is>
-          <t>ECMP</t>
-        </is>
-      </c>
-      <c r="D40" s="1" t="inlineStr">
-        <is>
-          <t>ECMP+SRv6</t>
-        </is>
-      </c>
-      <c r="E40" s="1" t="inlineStr">
-        <is>
-          <t>Variation1 (%)</t>
-        </is>
-      </c>
-      <c r="F40" s="1" t="inlineStr">
-        <is>
-          <t>Variation2 (%)</t>
-        </is>
-      </c>
-      <c r="G40" s="1" t="inlineStr">
-        <is>
-          <t>Variation3 (%)</t>
-        </is>
+          <t>Variation of the AVG 1º Packet Delay between (No)Emergency Flows (nanoseconds)</t>
+        </is>
+      </c>
+      <c r="B40">
+        <f>'HIGH-KShort'!D269</f>
+        <v/>
+      </c>
+      <c r="C40">
+        <f>'HIGH-ECMP'!D269</f>
+        <v/>
+      </c>
+      <c r="D40">
+        <f>'HIGH-ECMP-SRv6'!D330</f>
+        <v/>
+      </c>
+      <c r="E40">
+        <f>IFERROR(ROUND((C40 - B40) / B40 * 100, 3), 0)</f>
+        <v/>
+      </c>
+      <c r="F40">
+        <f>IFERROR(ROUND((D40 - B40) / B40 * 100, 3), 0)</f>
+        <v/>
+      </c>
+      <c r="G40">
+        <f>IFERROR(ROUND((D40 - C40) / C40 * 100, 3), 0)</f>
+        <v/>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>AVG Out of Order Packets (Nº)</t>
+          <t>Variation of the AVG Flow Delay between (No)Emergency Flows (nanoseconds)</t>
         </is>
       </c>
       <c r="B41">
-        <f>'HIGH+EMERGENCY-KShort'!B286</f>
+        <f>'HIGH-KShort'!D293</f>
         <v/>
       </c>
       <c r="C41">
-        <f>'HIGH+EMERGENCY-ECMP'!B286</f>
+        <f>'HIGH-ECMP'!D294</f>
         <v/>
       </c>
       <c r="D41">
-        <f>'HIGH+EMERGENCY-ECMP-SRv6'!B337</f>
+        <f>'HIGH-ECMP-SRv6'!D356</f>
         <v/>
       </c>
       <c r="E41">
@@ -5342,115 +5396,61 @@
         <v/>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" s="1" t="inlineStr">
-        <is>
-          <t>AVG Packet Loss (Nº)</t>
-        </is>
-      </c>
-      <c r="B42">
-        <f>'HIGH+EMERGENCY-KShort'!B287</f>
-        <v/>
-      </c>
-      <c r="C42">
-        <f>'HIGH+EMERGENCY-ECMP'!B287</f>
-        <v/>
-      </c>
-      <c r="D42">
-        <f>'HIGH+EMERGENCY-ECMP-SRv6'!B338</f>
-        <v/>
-      </c>
-      <c r="E42">
-        <f>IFERROR(ROUND((C42 - B42) / B42 * 100, 3), 0)</f>
-        <v/>
-      </c>
-      <c r="F42">
-        <f>IFERROR(ROUND((D42 - B42) / B42 * 100, 3), 0)</f>
-        <v/>
-      </c>
-      <c r="G42">
-        <f>IFERROR(ROUND((D42 - C42) / C42 * 100, 3), 0)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="1" t="inlineStr">
-        <is>
-          <t>AVG Packet Loss (%)</t>
-        </is>
-      </c>
-      <c r="B43">
-        <f>'HIGH+EMERGENCY-KShort'!B288</f>
-        <v/>
-      </c>
-      <c r="C43">
-        <f>'HIGH+EMERGENCY-ECMP'!B288</f>
-        <v/>
-      </c>
-      <c r="D43">
-        <f>'HIGH+EMERGENCY-ECMP-SRv6'!B339</f>
-        <v/>
-      </c>
-      <c r="E43">
-        <f>IFERROR(ROUND((C43 - B43) / B43 * 100, 3), 0)</f>
-        <v/>
-      </c>
-      <c r="F43">
-        <f>IFERROR(ROUND((D43 - B43) / B43 * 100, 3), 0)</f>
-        <v/>
-      </c>
-      <c r="G43">
-        <f>IFERROR(ROUND((D43 - C43) / C43 * 100, 3), 0)</f>
-        <v/>
-      </c>
-    </row>
+    <row r="42"/>
+    <row r="43"/>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>AVG 1º Packet Delay (nanoseconds)</t>
-        </is>
-      </c>
-      <c r="B44">
-        <f>'HIGH+EMERGENCY-KShort'!B289</f>
-        <v/>
-      </c>
-      <c r="C44">
-        <f>'HIGH+EMERGENCY-ECMP'!B289</f>
-        <v/>
-      </c>
-      <c r="D44">
-        <f>'HIGH+EMERGENCY-ECMP-SRv6'!B340</f>
-        <v/>
-      </c>
-      <c r="E44">
-        <f>IFERROR(ROUND((C44 - B44) / B44 * 100, 3), 0)</f>
-        <v/>
-      </c>
-      <c r="F44">
-        <f>IFERROR(ROUND((D44 - B44) / B44 * 100, 3), 0)</f>
-        <v/>
-      </c>
-      <c r="G44">
-        <f>IFERROR(ROUND((D44 - C44) / C44 * 100, 3), 0)</f>
-        <v/>
+          <t>HIGH+EMERGENCY</t>
+        </is>
+      </c>
+      <c r="B44" s="1" t="inlineStr">
+        <is>
+          <t>KShort</t>
+        </is>
+      </c>
+      <c r="C44" s="1" t="inlineStr">
+        <is>
+          <t>ECMP</t>
+        </is>
+      </c>
+      <c r="D44" s="1" t="inlineStr">
+        <is>
+          <t>ECMP+SRv6</t>
+        </is>
+      </c>
+      <c r="E44" s="1" t="inlineStr">
+        <is>
+          <t>Variation1 (%)</t>
+        </is>
+      </c>
+      <c r="F44" s="1" t="inlineStr">
+        <is>
+          <t>Variation2 (%)</t>
+        </is>
+      </c>
+      <c r="G44" s="1" t="inlineStr">
+        <is>
+          <t>Variation3 (%)</t>
+        </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>AVG Nº of SRv6 rules Created</t>
+          <t>AVG Out of Order Packets (Nº)</t>
         </is>
       </c>
       <c r="B45">
-        <f>'HIGH+EMERGENCY-KShort'!B290</f>
+        <f>'HIGH+EMERGENCY-KShort'!B286</f>
         <v/>
       </c>
       <c r="C45">
-        <f>'HIGH+EMERGENCY-ECMP'!B290</f>
+        <f>'HIGH+EMERGENCY-ECMP'!B286</f>
         <v/>
       </c>
       <c r="D45">
-        <f>'HIGH+EMERGENCY-ECMP-SRv6'!B341</f>
+        <f>'HIGH+EMERGENCY-ECMP-SRv6'!B337</f>
         <v/>
       </c>
       <c r="E45">
@@ -5469,19 +5469,19 @@
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>AVG Nº of SRv6 rules Removed</t>
+          <t>AVG Packet Loss (Nº)</t>
         </is>
       </c>
       <c r="B46">
-        <f>'HIGH+EMERGENCY-KShort'!B291</f>
+        <f>'HIGH+EMERGENCY-KShort'!B287</f>
         <v/>
       </c>
       <c r="C46">
-        <f>'HIGH+EMERGENCY-ECMP'!B291</f>
+        <f>'HIGH+EMERGENCY-ECMP'!B287</f>
         <v/>
       </c>
       <c r="D46">
-        <f>'HIGH+EMERGENCY-ECMP-SRv6'!B342</f>
+        <f>'HIGH+EMERGENCY-ECMP-SRv6'!B338</f>
         <v/>
       </c>
       <c r="E46">
@@ -5500,19 +5500,19 @@
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>AVG Flows Latency (nanoseconds)</t>
+          <t>AVG Packet Loss (%)</t>
         </is>
       </c>
       <c r="B47">
-        <f>'HIGH+EMERGENCY-KShort'!B292</f>
+        <f>'HIGH+EMERGENCY-KShort'!B288</f>
         <v/>
       </c>
       <c r="C47">
-        <f>'HIGH+EMERGENCY-ECMP'!B292</f>
+        <f>'HIGH+EMERGENCY-ECMP'!B288</f>
         <v/>
       </c>
       <c r="D47">
-        <f>'HIGH+EMERGENCY-ECMP-SRv6'!B343</f>
+        <f>'HIGH+EMERGENCY-ECMP-SRv6'!B339</f>
         <v/>
       </c>
       <c r="E47">
@@ -5531,19 +5531,19 @@
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>AVG Hop Latency (nanoseconds)</t>
+          <t>AVG 1º Packet Delay (nanoseconds)</t>
         </is>
       </c>
       <c r="B48">
-        <f>'HIGH+EMERGENCY-KShort'!B294</f>
+        <f>'HIGH+EMERGENCY-KShort'!B289</f>
         <v/>
       </c>
       <c r="C48">
-        <f>'HIGH+EMERGENCY-ECMP'!B294</f>
+        <f>'HIGH+EMERGENCY-ECMP'!B289</f>
         <v/>
       </c>
       <c r="D48">
-        <f>'HIGH+EMERGENCY-ECMP-SRv6'!B345</f>
+        <f>'HIGH+EMERGENCY-ECMP-SRv6'!B340</f>
         <v/>
       </c>
       <c r="E48">
@@ -5562,19 +5562,19 @@
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>AVG of packets to each switch (%)</t>
+          <t>AVG Nº of SRv6 rules Created</t>
         </is>
       </c>
       <c r="B49">
-        <f>'HIGH+EMERGENCY-KShort'!B307</f>
+        <f>'HIGH+EMERGENCY-KShort'!B290</f>
         <v/>
       </c>
       <c r="C49">
-        <f>'HIGH+EMERGENCY-ECMP'!B310</f>
+        <f>'HIGH+EMERGENCY-ECMP'!B290</f>
         <v/>
       </c>
       <c r="D49">
-        <f>'HIGH+EMERGENCY-ECMP-SRv6'!B361</f>
+        <f>'HIGH+EMERGENCY-ECMP-SRv6'!B341</f>
         <v/>
       </c>
       <c r="E49">
@@ -5593,19 +5593,19 @@
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>Standard Deviation of packets to each switch (%)</t>
+          <t>AVG Nº of SRv6 rules Removed</t>
         </is>
       </c>
       <c r="B50">
-        <f>'HIGH+EMERGENCY-KShort'!B308</f>
+        <f>'HIGH+EMERGENCY-KShort'!B291</f>
         <v/>
       </c>
       <c r="C50">
-        <f>'HIGH+EMERGENCY-ECMP'!B311</f>
+        <f>'HIGH+EMERGENCY-ECMP'!B291</f>
         <v/>
       </c>
       <c r="D50">
-        <f>'HIGH+EMERGENCY-ECMP-SRv6'!B362</f>
+        <f>'HIGH+EMERGENCY-ECMP-SRv6'!B342</f>
         <v/>
       </c>
       <c r="E50">
@@ -5624,19 +5624,19 @@
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>AVG of processed Bytes to each switch</t>
+          <t>AVG Flows Latency (nanoseconds)</t>
         </is>
       </c>
       <c r="B51">
-        <f>'HIGH+EMERGENCY-KShort'!C307</f>
+        <f>'HIGH+EMERGENCY-KShort'!B292</f>
         <v/>
       </c>
       <c r="C51">
-        <f>'HIGH+EMERGENCY-ECMP'!C310</f>
+        <f>'HIGH+EMERGENCY-ECMP'!B292</f>
         <v/>
       </c>
       <c r="D51">
-        <f>'HIGH+EMERGENCY-ECMP-SRv6'!C361</f>
+        <f>'HIGH+EMERGENCY-ECMP-SRv6'!B343</f>
         <v/>
       </c>
       <c r="E51">
@@ -5655,19 +5655,19 @@
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>Standard Deviation of processed Bytes to each switch</t>
+          <t>STD Flows Latency (nanoseconds)</t>
         </is>
       </c>
       <c r="B52">
-        <f>'HIGH+EMERGENCY-KShort'!C308</f>
+        <f>'HIGH+EMERGENCY-KShort'!B293</f>
         <v/>
       </c>
       <c r="C52">
-        <f>'HIGH+EMERGENCY-ECMP'!C311</f>
+        <f>'HIGH+EMERGENCY-ECMP'!B293</f>
         <v/>
       </c>
       <c r="D52">
-        <f>'HIGH+EMERGENCY-ECMP-SRv6'!C362</f>
+        <f>'HIGH+EMERGENCY-ECMP-SRv6'!B344</f>
         <v/>
       </c>
       <c r="E52">
@@ -5686,19 +5686,19 @@
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>Variation of the AVG 1º Packet Delay between (No)Emergency Flows (nanoseconds)</t>
+          <t>AVG Hop Latency (nanoseconds)</t>
         </is>
       </c>
       <c r="B53">
-        <f>'HIGH+EMERGENCY-KShort'!D311</f>
+        <f>'HIGH+EMERGENCY-KShort'!B294</f>
         <v/>
       </c>
       <c r="C53">
-        <f>'HIGH+EMERGENCY-ECMP'!D314</f>
+        <f>'HIGH+EMERGENCY-ECMP'!B294</f>
         <v/>
       </c>
       <c r="D53">
-        <f>'HIGH+EMERGENCY-ECMP-SRv6'!D365</f>
+        <f>'HIGH+EMERGENCY-ECMP-SRv6'!B345</f>
         <v/>
       </c>
       <c r="E53">
@@ -5717,19 +5717,19 @@
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>Variation of the AVG Flow Delay between (No)Emergency Flows (nanoseconds)</t>
+          <t>STD Hop Latency (nanoseconds)</t>
         </is>
       </c>
       <c r="B54">
-        <f>'HIGH+EMERGENCY-KShort'!D312</f>
+        <f>'HIGH+EMERGENCY-KShort'!B295</f>
         <v/>
       </c>
       <c r="C54">
-        <f>'HIGH+EMERGENCY-ECMP'!D315</f>
+        <f>'HIGH+EMERGENCY-ECMP'!B295</f>
         <v/>
       </c>
       <c r="D54">
-        <f>'HIGH+EMERGENCY-ECMP-SRv6'!D366</f>
+        <f>'HIGH+EMERGENCY-ECMP-SRv6'!B346</f>
         <v/>
       </c>
       <c r="E54">
@@ -5745,8 +5745,194 @@
         <v/>
       </c>
     </row>
-    <row r="55"/>
-    <row r="56"/>
+    <row r="55">
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t>AVG of packets to each switch (%)</t>
+        </is>
+      </c>
+      <c r="B55">
+        <f>'HIGH+EMERGENCY-KShort'!C307</f>
+        <v/>
+      </c>
+      <c r="C55">
+        <f>'HIGH+EMERGENCY-ECMP'!C310</f>
+        <v/>
+      </c>
+      <c r="D55">
+        <f>'HIGH+EMERGENCY-ECMP-SRv6'!C361</f>
+        <v/>
+      </c>
+      <c r="E55">
+        <f>IFERROR(ROUND((C55 - B55) / B55 * 100, 3), 0)</f>
+        <v/>
+      </c>
+      <c r="F55">
+        <f>IFERROR(ROUND((D55 - B55) / B55 * 100, 3), 0)</f>
+        <v/>
+      </c>
+      <c r="G55">
+        <f>IFERROR(ROUND((D55 - C55) / C55 * 100, 3), 0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t>Standard Deviation of packets to each switch (%)</t>
+        </is>
+      </c>
+      <c r="B56">
+        <f>'HIGH+EMERGENCY-KShort'!C308</f>
+        <v/>
+      </c>
+      <c r="C56">
+        <f>'HIGH+EMERGENCY-ECMP'!C311</f>
+        <v/>
+      </c>
+      <c r="D56">
+        <f>'HIGH+EMERGENCY-ECMP-SRv6'!C362</f>
+        <v/>
+      </c>
+      <c r="E56">
+        <f>IFERROR(ROUND((C56 - B56) / B56 * 100, 3), 0)</f>
+        <v/>
+      </c>
+      <c r="F56">
+        <f>IFERROR(ROUND((D56 - B56) / B56 * 100, 3), 0)</f>
+        <v/>
+      </c>
+      <c r="G56">
+        <f>IFERROR(ROUND((D56 - C56) / C56 * 100, 3), 0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="inlineStr">
+        <is>
+          <t>AVG of processed Bytes to each switch</t>
+        </is>
+      </c>
+      <c r="B57">
+        <f>'HIGH+EMERGENCY-KShort'!C307</f>
+        <v/>
+      </c>
+      <c r="C57">
+        <f>'HIGH+EMERGENCY-ECMP'!C310</f>
+        <v/>
+      </c>
+      <c r="D57">
+        <f>'HIGH+EMERGENCY-ECMP-SRv6'!C361</f>
+        <v/>
+      </c>
+      <c r="E57">
+        <f>IFERROR(ROUND((C57 - B57) / B57 * 100, 3), 0)</f>
+        <v/>
+      </c>
+      <c r="F57">
+        <f>IFERROR(ROUND((D57 - B57) / B57 * 100, 3), 0)</f>
+        <v/>
+      </c>
+      <c r="G57">
+        <f>IFERROR(ROUND((D57 - C57) / C57 * 100, 3), 0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t>Standard Deviation of processed Bytes to each switch</t>
+        </is>
+      </c>
+      <c r="B58">
+        <f>'HIGH+EMERGENCY-KShort'!C308</f>
+        <v/>
+      </c>
+      <c r="C58">
+        <f>'HIGH+EMERGENCY-ECMP'!C311</f>
+        <v/>
+      </c>
+      <c r="D58">
+        <f>'HIGH+EMERGENCY-ECMP-SRv6'!C362</f>
+        <v/>
+      </c>
+      <c r="E58">
+        <f>IFERROR(ROUND((C58 - B58) / B58 * 100, 3), 0)</f>
+        <v/>
+      </c>
+      <c r="F58">
+        <f>IFERROR(ROUND((D58 - B58) / B58 * 100, 3), 0)</f>
+        <v/>
+      </c>
+      <c r="G58">
+        <f>IFERROR(ROUND((D58 - C58) / C58 * 100, 3), 0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="inlineStr">
+        <is>
+          <t>Variation of the AVG 1º Packet Delay between (No)Emergency Flows (nanoseconds)</t>
+        </is>
+      </c>
+      <c r="B59">
+        <f>'HIGH+EMERGENCY-KShort'!D289</f>
+        <v/>
+      </c>
+      <c r="C59">
+        <f>'HIGH+EMERGENCY-ECMP'!D289</f>
+        <v/>
+      </c>
+      <c r="D59">
+        <f>'HIGH+EMERGENCY-ECMP-SRv6'!D340</f>
+        <v/>
+      </c>
+      <c r="E59">
+        <f>IFERROR(ROUND((C59 - B59) / B59 * 100, 3), 0)</f>
+        <v/>
+      </c>
+      <c r="F59">
+        <f>IFERROR(ROUND((D59 - B59) / B59 * 100, 3), 0)</f>
+        <v/>
+      </c>
+      <c r="G59">
+        <f>IFERROR(ROUND((D59 - C59) / C59 * 100, 3), 0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="inlineStr">
+        <is>
+          <t>Variation of the AVG Flow Delay between (No)Emergency Flows (nanoseconds)</t>
+        </is>
+      </c>
+      <c r="B60">
+        <f>'HIGH+EMERGENCY-KShort'!D312</f>
+        <v/>
+      </c>
+      <c r="C60">
+        <f>'HIGH+EMERGENCY-ECMP'!D315</f>
+        <v/>
+      </c>
+      <c r="D60">
+        <f>'HIGH+EMERGENCY-ECMP-SRv6'!D366</f>
+        <v/>
+      </c>
+      <c r="E60">
+        <f>IFERROR(ROUND((C60 - B60) / B60 * 100, 3), 0)</f>
+        <v/>
+      </c>
+      <c r="F60">
+        <f>IFERROR(ROUND((D60 - B60) / B60 * 100, 3), 0)</f>
+        <v/>
+      </c>
+      <c r="G60">
+        <f>IFERROR(ROUND((D60 - C60) / C60 * 100, 3), 0)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="61"/>
+    <row r="62"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed wrong values being copied
</commit_message>
<xml_diff>
--- a/INT/results/final_results.xlsx
+++ b/INT/results/final_results.xlsx
@@ -4682,15 +4682,15 @@
         </is>
       </c>
       <c r="B17">
-        <f>'MEDIUM-KShort'!C126</f>
+        <f>'MEDIUM-KShort'!B126</f>
         <v/>
       </c>
       <c r="C17">
-        <f>'MEDIUM-ECMP'!C129</f>
+        <f>'MEDIUM-ECMP'!B129</f>
         <v/>
       </c>
       <c r="D17">
-        <f>'MEDIUM-ECMP-SRv6'!C128</f>
+        <f>'MEDIUM-ECMP-SRv6'!B128</f>
         <v/>
       </c>
       <c r="E17">
@@ -4713,15 +4713,15 @@
         </is>
       </c>
       <c r="B18">
-        <f>'MEDIUM-KShort'!C127</f>
+        <f>'MEDIUM-KShort'!B127</f>
         <v/>
       </c>
       <c r="C18">
-        <f>'MEDIUM-ECMP'!C130</f>
+        <f>'MEDIUM-ECMP'!B130</f>
         <v/>
       </c>
       <c r="D18">
-        <f>'MEDIUM-ECMP-SRv6'!C129</f>
+        <f>'MEDIUM-ECMP-SRv6'!B129</f>
         <v/>
       </c>
       <c r="E18">
@@ -4806,15 +4806,15 @@
         </is>
       </c>
       <c r="B21">
-        <f>'MEDIUM-KShort'!D109</f>
+        <f>'MEDIUM-KShort'!D130</f>
         <v/>
       </c>
       <c r="C21">
-        <f>'MEDIUM-ECMP'!D109</f>
+        <f>'MEDIUM-ECMP'!D133</f>
         <v/>
       </c>
       <c r="D21">
-        <f>'MEDIUM-ECMP-SRv6'!D109</f>
+        <f>'MEDIUM-ECMP-SRv6'!D132</f>
         <v/>
       </c>
       <c r="E21">
@@ -5217,15 +5217,15 @@
         </is>
       </c>
       <c r="B36">
-        <f>'HIGH-KShort'!C288</f>
+        <f>'HIGH-KShort'!B288</f>
         <v/>
       </c>
       <c r="C36">
-        <f>'HIGH-ECMP'!C289</f>
+        <f>'HIGH-ECMP'!B289</f>
         <v/>
       </c>
       <c r="D36">
-        <f>'HIGH-ECMP-SRv6'!C351</f>
+        <f>'HIGH-ECMP-SRv6'!B351</f>
         <v/>
       </c>
       <c r="E36">
@@ -5248,15 +5248,15 @@
         </is>
       </c>
       <c r="B37">
-        <f>'HIGH-KShort'!C289</f>
+        <f>'HIGH-KShort'!B289</f>
         <v/>
       </c>
       <c r="C37">
-        <f>'HIGH-ECMP'!C290</f>
+        <f>'HIGH-ECMP'!B290</f>
         <v/>
       </c>
       <c r="D37">
-        <f>'HIGH-ECMP-SRv6'!C352</f>
+        <f>'HIGH-ECMP-SRv6'!B352</f>
         <v/>
       </c>
       <c r="E37">
@@ -5341,15 +5341,15 @@
         </is>
       </c>
       <c r="B40">
-        <f>'HIGH-KShort'!D269</f>
+        <f>'HIGH-KShort'!D292</f>
         <v/>
       </c>
       <c r="C40">
-        <f>'HIGH-ECMP'!D269</f>
+        <f>'HIGH-ECMP'!D293</f>
         <v/>
       </c>
       <c r="D40">
-        <f>'HIGH-ECMP-SRv6'!D330</f>
+        <f>'HIGH-ECMP-SRv6'!D355</f>
         <v/>
       </c>
       <c r="E40">
@@ -5752,15 +5752,15 @@
         </is>
       </c>
       <c r="B55">
-        <f>'HIGH+EMERGENCY-KShort'!C307</f>
+        <f>'HIGH+EMERGENCY-KShort'!B307</f>
         <v/>
       </c>
       <c r="C55">
-        <f>'HIGH+EMERGENCY-ECMP'!C310</f>
+        <f>'HIGH+EMERGENCY-ECMP'!B310</f>
         <v/>
       </c>
       <c r="D55">
-        <f>'HIGH+EMERGENCY-ECMP-SRv6'!C361</f>
+        <f>'HIGH+EMERGENCY-ECMP-SRv6'!B361</f>
         <v/>
       </c>
       <c r="E55">
@@ -5783,15 +5783,15 @@
         </is>
       </c>
       <c r="B56">
-        <f>'HIGH+EMERGENCY-KShort'!C308</f>
+        <f>'HIGH+EMERGENCY-KShort'!B308</f>
         <v/>
       </c>
       <c r="C56">
-        <f>'HIGH+EMERGENCY-ECMP'!C311</f>
+        <f>'HIGH+EMERGENCY-ECMP'!B311</f>
         <v/>
       </c>
       <c r="D56">
-        <f>'HIGH+EMERGENCY-ECMP-SRv6'!C362</f>
+        <f>'HIGH+EMERGENCY-ECMP-SRv6'!B362</f>
         <v/>
       </c>
       <c r="E56">
@@ -5876,15 +5876,15 @@
         </is>
       </c>
       <c r="B59">
-        <f>'HIGH+EMERGENCY-KShort'!D289</f>
+        <f>'HIGH+EMERGENCY-KShort'!D311</f>
         <v/>
       </c>
       <c r="C59">
-        <f>'HIGH+EMERGENCY-ECMP'!D289</f>
+        <f>'HIGH+EMERGENCY-ECMP'!D314</f>
         <v/>
       </c>
       <c r="D59">
-        <f>'HIGH+EMERGENCY-ECMP-SRv6'!D340</f>
+        <f>'HIGH+EMERGENCY-ECMP-SRv6'!D365</f>
         <v/>
       </c>
       <c r="E59">

</xml_diff>

<commit_message>
now excluding latency values over percentil of 95 %
</commit_message>
<xml_diff>
--- a/INT/results/final_results.xlsx
+++ b/INT/results/final_results.xlsx
@@ -4045,7 +4045,7 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>37684.91</v>
+        <v>36485.444</v>
       </c>
     </row>
     <row r="113">
@@ -4055,7 +4055,7 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>21098.839</v>
+        <v>20621.508</v>
       </c>
     </row>
     <row r="114">
@@ -4065,7 +4065,7 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>1809.493</v>
+        <v>1788.752</v>
       </c>
     </row>
     <row r="115">
@@ -4075,7 +4075,7 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>2511.087</v>
+        <v>1333.168</v>
       </c>
     </row>
     <row r="116"/>
@@ -16283,7 +16283,7 @@
         </is>
       </c>
       <c r="B272" t="n">
-        <v>30146.111</v>
+        <v>28802.893</v>
       </c>
     </row>
     <row r="273">
@@ -16293,7 +16293,7 @@
         </is>
       </c>
       <c r="B273" t="n">
-        <v>17172.786</v>
+        <v>16513.672</v>
       </c>
     </row>
     <row r="274">
@@ -16303,7 +16303,7 @@
         </is>
       </c>
       <c r="B274" t="n">
-        <v>2108.911</v>
+        <v>2104.547</v>
       </c>
     </row>
     <row r="275">
@@ -16313,7 +16313,7 @@
         </is>
       </c>
       <c r="B275" t="n">
-        <v>1719.756</v>
+        <v>1624.644</v>
       </c>
     </row>
     <row r="276"/>
@@ -27721,7 +27721,7 @@
         </is>
       </c>
       <c r="B292" t="n">
-        <v>12212.473</v>
+        <v>11393.111</v>
       </c>
     </row>
     <row r="293">
@@ -27731,7 +27731,7 @@
         </is>
       </c>
       <c r="B293" t="n">
-        <v>5887.902</v>
+        <v>4397.78</v>
       </c>
     </row>
     <row r="294">
@@ -27741,7 +27741,7 @@
         </is>
       </c>
       <c r="B294" t="n">
-        <v>2212.144</v>
+        <v>2200.092</v>
       </c>
     </row>
     <row r="295">
@@ -27751,7 +27751,7 @@
         </is>
       </c>
       <c r="B295" t="n">
-        <v>1833.306</v>
+        <v>1658.718</v>
       </c>
     </row>
     <row r="296"/>
@@ -31586,7 +31586,7 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>39236.592</v>
+        <v>38510.118</v>
       </c>
     </row>
     <row r="113">
@@ -31596,7 +31596,7 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>18734.157</v>
+        <v>18937.641</v>
       </c>
     </row>
     <row r="114">
@@ -31606,7 +31606,7 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>1626.079</v>
+        <v>1624.868</v>
       </c>
     </row>
     <row r="115">
@@ -31616,7 +31616,7 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>1053.113</v>
+        <v>1006.025</v>
       </c>
     </row>
     <row r="116"/>
@@ -42195,7 +42195,7 @@
         </is>
       </c>
       <c r="B272" t="n">
-        <v>11422.341</v>
+        <v>10644.981</v>
       </c>
     </row>
     <row r="273">
@@ -42205,7 +42205,7 @@
         </is>
       </c>
       <c r="B273" t="n">
-        <v>5704.176</v>
+        <v>4436.355</v>
       </c>
     </row>
     <row r="274">
@@ -42215,7 +42215,7 @@
         </is>
       </c>
       <c r="B274" t="n">
-        <v>2057.99</v>
+        <v>2046.413</v>
       </c>
     </row>
     <row r="275">
@@ -42225,7 +42225,7 @@
         </is>
       </c>
       <c r="B275" t="n">
-        <v>1637.912</v>
+        <v>1500.807</v>
       </c>
     </row>
     <row r="276"/>
@@ -53644,7 +53644,7 @@
         </is>
       </c>
       <c r="B292" t="n">
-        <v>12341.561</v>
+        <v>11551.028</v>
       </c>
     </row>
     <row r="293">
@@ -53654,7 +53654,7 @@
         </is>
       </c>
       <c r="B293" t="n">
-        <v>5776.884</v>
+        <v>4258.377</v>
       </c>
     </row>
     <row r="294">
@@ -53664,7 +53664,7 @@
         </is>
       </c>
       <c r="B294" t="n">
-        <v>2217.331</v>
+        <v>2203.989</v>
       </c>
     </row>
     <row r="295">
@@ -53674,7 +53674,7 @@
         </is>
       </c>
       <c r="B295" t="n">
-        <v>1859.99</v>
+        <v>1611.968</v>
       </c>
     </row>
     <row r="296"/>
@@ -57542,7 +57542,7 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>40401.129</v>
+        <v>39419.877</v>
       </c>
     </row>
     <row r="113">
@@ -57552,7 +57552,7 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>19559.673</v>
+        <v>18858.446</v>
       </c>
     </row>
     <row r="114">
@@ -57562,7 +57562,7 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>1593.881</v>
+        <v>1562.227</v>
       </c>
     </row>
     <row r="115">
@@ -57572,7 +57572,7 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>3043.343</v>
+        <v>1042.793</v>
       </c>
     </row>
     <row r="116"/>
@@ -69165,7 +69165,7 @@
         </is>
       </c>
       <c r="B333" t="n">
-        <v>12636.655</v>
+        <v>11778.849</v>
       </c>
     </row>
     <row r="334">
@@ -69175,7 +69175,7 @@
         </is>
       </c>
       <c r="B334" t="n">
-        <v>6074.242</v>
+        <v>4531.333</v>
       </c>
     </row>
     <row r="335">
@@ -69185,7 +69185,7 @@
         </is>
       </c>
       <c r="B335" t="n">
-        <v>2220.584</v>
+        <v>2207.862</v>
       </c>
     </row>
     <row r="336">
@@ -69195,7 +69195,7 @@
         </is>
       </c>
       <c r="B336" t="n">
-        <v>1898.614</v>
+        <v>1720.607</v>
       </c>
     </row>
     <row r="337"/>
@@ -81370,7 +81370,7 @@
         </is>
       </c>
       <c r="B343" t="n">
-        <v>12456.195</v>
+        <v>11525.61</v>
       </c>
     </row>
     <row r="344">
@@ -81380,7 +81380,7 @@
         </is>
       </c>
       <c r="B344" t="n">
-        <v>10473.906</v>
+        <v>4303.685</v>
       </c>
     </row>
     <row r="345">
@@ -81390,7 +81390,7 @@
         </is>
       </c>
       <c r="B345" t="n">
-        <v>2216.623</v>
+        <v>2169.462</v>
       </c>
     </row>
     <row r="346">
@@ -81400,7 +81400,7 @@
         </is>
       </c>
       <c r="B346" t="n">
-        <v>4196.799</v>
+        <v>1629.03</v>
       </c>
     </row>
     <row r="347"/>

</xml_diff>